<commit_message>
new functions to test
git-svn-id: https://xp-dev.com/svn/LS_Tools/trunk@36 5f53ba06-53dd-4be5-a6e0-4a502202dc76
</commit_message>
<xml_diff>
--- a/Excel2Code/test.xlsx
+++ b/Excel2Code/test.xlsx
@@ -14,17 +14,19 @@
   <definedNames>
     <definedName name="cube">Sheet1!$E$3</definedName>
     <definedName name="cube_sqrt">Sheet1!$F$3</definedName>
+    <definedName name="is_even">Sheet1!$I$3</definedName>
+    <definedName name="log_cube">Sheet1!$K$3</definedName>
     <definedName name="mult">Sheet1!$G$3</definedName>
+    <definedName name="repeat_line">Sheet1!$J$3</definedName>
     <definedName name="square">Sheet1!$D$3</definedName>
     <definedName name="times2">Sheet1!$H$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:Q13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -45,6 +47,15 @@
   </si>
   <si>
     <t>times2</t>
+  </si>
+  <si>
+    <t>is even?</t>
+  </si>
+  <si>
+    <t>repeat</t>
+  </si>
+  <si>
+    <t>log_cube</t>
   </si>
 </sst>
 </file>
@@ -383,18 +394,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -416,8 +428,17 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -444,8 +465,20 @@
         <f>B3*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="str">
+        <f>IF(MOD(B3,2)=0,"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="J3" t="str">
+        <f>REPT("|",G3)</f>
+        <v>|||||||||</v>
+      </c>
+      <c r="K3">
+        <f>LOG10(E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -472,8 +505,20 @@
         <f t="shared" ref="H4:H12" si="4">B4*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I12" si="5">IF(MOD(B4,2)=0,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J12" si="6">REPT("|",G4)</f>
+        <v>||||||||||||||||</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K12" si="7">LOG10(E4)</f>
+        <v>0.90308998699194354</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -500,8 +545,20 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="6"/>
+        <v>|||||||||||||||||||||</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="7"/>
+        <v>1.4313637641589874</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -528,8 +585,20 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v>||||||||||||||||||||||||</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="7"/>
+        <v>1.8061799739838871</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -556,8 +625,20 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>|||||||||||||||||||||||||</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="7"/>
+        <v>2.0969100130080562</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -584,8 +665,20 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v>||||||||||||||||||||||||</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>2.3344537511509307</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
@@ -612,8 +705,20 @@
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v>|||||||||||||||||||||</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="7"/>
+        <v>2.5352941200427703</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
@@ -640,8 +745,20 @@
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v>||||||||||||||||</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>2.7092699609758308</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
@@ -668,8 +785,20 @@
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v>|||||||||</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="7"/>
+        <v>2.8627275283179747</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -695,6 +824,18 @@
       <c r="H12">
         <f t="shared" si="4"/>
         <v>20</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="K12">
+        <f t="shared" si="7"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>